<commit_message>
Successfully tested 'Partial Volume Estimation' using my own imaging and spectroscopy data
</commit_message>
<xml_diff>
--- a/t_stats.xlsx
+++ b/t_stats.xlsx
@@ -113,139 +113,139 @@
     <t>X6</t>
   </si>
   <si>
-    <t>-8.76204864074198</t>
-  </si>
-  <si>
-    <t>-9.95394030652895</t>
-  </si>
-  <si>
-    <t>-9.25233562442458</t>
-  </si>
-  <si>
-    <t>-10.5638603544957</t>
-  </si>
-  <si>
-    <t>10.7580641399361</t>
-  </si>
-  <si>
-    <t>-1.31911515290534</t>
-  </si>
-  <si>
-    <t>-1.00231051109186</t>
-  </si>
-  <si>
-    <t>-1.94263777184821</t>
-  </si>
-  <si>
-    <t>27.7108211943028</t>
-  </si>
-  <si>
-    <t>0.234004010498296</t>
-  </si>
-  <si>
-    <t>-0.613579556846957</t>
-  </si>
-  <si>
-    <t>29.8993479597623</t>
-  </si>
-  <si>
-    <t>-0.809477403314938</t>
-  </si>
-  <si>
-    <t>26.1014566549566</t>
-  </si>
-  <si>
-    <t>31.3987228765185</t>
-  </si>
-  <si>
-    <t>89.1157456032421</t>
-  </si>
-  <si>
-    <t>88.6716584735645</t>
-  </si>
-  <si>
-    <t>92.5686947304437</t>
-  </si>
-  <si>
-    <t>87.8418899335703</t>
-  </si>
-  <si>
-    <t>47.6358127448591</t>
-  </si>
-  <si>
-    <t>93.987147095759</t>
-  </si>
-  <si>
-    <t>92.8136962015839</t>
-  </si>
-  <si>
-    <t>93.8996699281846</t>
-  </si>
-  <si>
-    <t>48.0244386309057</t>
-  </si>
-  <si>
-    <t>92.5632875627298</t>
-  </si>
-  <si>
-    <t>93.9585580568856</t>
-  </si>
-  <si>
-    <t>48.0486759215951</t>
-  </si>
-  <si>
-    <t>92.0589416396928</t>
-  </si>
-  <si>
-    <t>47.8163649500138</t>
-  </si>
-  <si>
-    <t>48.0936565992459</t>
-  </si>
-  <si>
-    <t>1.15643600360063e-13</t>
-  </si>
-  <si>
-    <t>4.13781798006722e-16</t>
-  </si>
-  <si>
-    <t>8.11847244537063e-15</t>
-  </si>
-  <si>
-    <t>2.57499356322772e-17</t>
-  </si>
-  <si>
-    <t>2.41901609951135e-14</t>
-  </si>
-  <si>
-    <t>0.190335411018389</t>
-  </si>
-  <si>
-    <t>0.31879966077825</t>
-  </si>
-  <si>
-    <t>0.0550558353486236</t>
-  </si>
-  <si>
-    <t>3.40546956746808e-31</t>
-  </si>
-  <si>
-    <t>0.815498648238359</t>
-  </si>
-  <si>
-    <t>0.540975806738249</t>
-  </si>
-  <si>
-    <t>1.05003500960804e-32</t>
-  </si>
-  <si>
-    <t>0.420327918645286</t>
-  </si>
-  <si>
-    <t>6.10313880441278e-30</t>
-  </si>
-  <si>
-    <t>1.06670987325226e-33</t>
+    <t>-10.9932194001311</t>
+  </si>
+  <si>
+    <t>-11.6321953539881</t>
+  </si>
+  <si>
+    <t>-15.0456482614919</t>
+  </si>
+  <si>
+    <t>-14.0743090735612</t>
+  </si>
+  <si>
+    <t>8.67946751904764</t>
+  </si>
+  <si>
+    <t>-0.420955880210163</t>
+  </si>
+  <si>
+    <t>-2.10316666421769</t>
+  </si>
+  <si>
+    <t>-0.867058542091472</t>
+  </si>
+  <si>
+    <t>21.5512730372604</t>
+  </si>
+  <si>
+    <t>-1.66411568527365</t>
+  </si>
+  <si>
+    <t>-0.394283509893122</t>
+  </si>
+  <si>
+    <t>22.7609488720519</t>
+  </si>
+  <si>
+    <t>1.52578747925203</t>
+  </si>
+  <si>
+    <t>31.8463419756661</t>
+  </si>
+  <si>
+    <t>31.9310224417696</t>
+  </si>
+  <si>
+    <t>64.0370307305784</t>
+  </si>
+  <si>
+    <t>64.5925315019376</t>
+  </si>
+  <si>
+    <t>65.3128771122382</t>
+  </si>
+  <si>
+    <t>64.0959410014433</t>
+  </si>
+  <si>
+    <t>34.0561802025822</t>
+  </si>
+  <si>
+    <t>65.9475693641348</t>
+  </si>
+  <si>
+    <t>61.4299622560178</t>
+  </si>
+  <si>
+    <t>59.2595615280683</t>
+  </si>
+  <si>
+    <t>33.7415444319119</t>
+  </si>
+  <si>
+    <t>62.22079215284</t>
+  </si>
+  <si>
+    <t>60.1441661965777</t>
+  </si>
+  <si>
+    <t>33.7845636403643</t>
+  </si>
+  <si>
+    <t>65.6685736360082</t>
+  </si>
+  <si>
+    <t>34.2974374030118</t>
+  </si>
+  <si>
+    <t>34.4956896545343</t>
+  </si>
+  <si>
+    <t>2.19856237737517e-16</t>
+  </si>
+  <si>
+    <t>1.70327372671198e-17</t>
+  </si>
+  <si>
+    <t>6.63883335973362e-23</t>
+  </si>
+  <si>
+    <t>2.81537071135295e-21</t>
+  </si>
+  <si>
+    <t>3.79206722649747e-10</t>
+  </si>
+  <si>
+    <t>0.675156044280717</t>
+  </si>
+  <si>
+    <t>0.0395545430011091</t>
+  </si>
+  <si>
+    <t>0.38940734031658</t>
+  </si>
+  <si>
+    <t>2.64877596791972e-21</t>
+  </si>
+  <si>
+    <t>0.101118166962509</t>
+  </si>
+  <si>
+    <t>0.694766337294604</t>
+  </si>
+  <si>
+    <t>4.52153999486825e-22</t>
+  </si>
+  <si>
+    <t>0.131864961649821</t>
+  </si>
+  <si>
+    <t>4.64458789074224e-27</t>
+  </si>
+  <si>
+    <t>3.32481233563374e-27</t>
   </si>
   <si>
     <t>Welch Two Sample t-test</t>
@@ -257,112 +257,112 @@
     <t>0</t>
   </si>
   <si>
-    <t>-27.6511389709457</t>
-  </si>
-  <si>
-    <t>-30.5812901155514</t>
-  </si>
-  <si>
-    <t>-30.2880527212741</t>
-  </si>
-  <si>
-    <t>-31.8934469543834</t>
-  </si>
-  <si>
-    <t>17.7350345905215</t>
-  </si>
-  <si>
-    <t>-7.39653003432014</t>
-  </si>
-  <si>
-    <t>-7.14306400907783</t>
-  </si>
-  <si>
-    <t>-8.7023404094842</t>
-  </si>
-  <si>
-    <t>41.1342824507789</t>
-  </si>
-  <si>
-    <t>-4.16636071062889</t>
-  </si>
-  <si>
-    <t>-5.72349723612422</t>
-  </si>
-  <si>
-    <t>44.123808440061</t>
-  </si>
-  <si>
-    <t>-6.58814660894923</t>
-  </si>
-  <si>
-    <t>43.1468700829126</t>
-  </si>
-  <si>
-    <t>45.5404262440208</t>
-  </si>
-  <si>
-    <t>-17.4285540025109</t>
-  </si>
-  <si>
-    <t>-20.4033538025195</t>
-  </si>
-  <si>
-    <t>-19.5835901453594</t>
-  </si>
-  <si>
-    <t>-21.793518089974</t>
-  </si>
-  <si>
-    <t>25.8899654094785</t>
-  </si>
-  <si>
-    <t>1.49157908970575</t>
-  </si>
-  <si>
-    <t>2.3511141159008</t>
-  </si>
-  <si>
-    <t>0.0950683385833255</t>
-  </si>
-  <si>
-    <t>47.5704105226777</t>
-  </si>
-  <si>
-    <t>5.27936176206624</t>
-  </si>
-  <si>
-    <t>3.02117610983773</t>
-  </si>
-  <si>
-    <t>50.4858354780099</t>
-  </si>
-  <si>
-    <t>2.77282443122539</t>
-  </si>
-  <si>
-    <t>50.349772783721</t>
-  </si>
-  <si>
-    <t>51.7715388003366</t>
-  </si>
-  <si>
-    <t>24.5</t>
-  </si>
-  <si>
-    <t>47.0398464867283</t>
-  </si>
-  <si>
-    <t>49.9923219590355</t>
-  </si>
-  <si>
-    <t>49.4358214333168</t>
-  </si>
-  <si>
-    <t>51.3434825221787</t>
-  </si>
-  <si>
-    <t>2.6875</t>
+    <t>-34.5456291467162</t>
+  </si>
+  <si>
+    <t>-35.6551707539455</t>
+  </si>
+  <si>
+    <t>-39.2004817069638</t>
+  </si>
+  <si>
+    <t>-35.8507432583315</t>
+  </si>
+  <si>
+    <t>11.4430034686036</t>
+  </si>
+  <si>
+    <t>-6.87265354461256</t>
+  </si>
+  <si>
+    <t>-10.482486160765</t>
+  </si>
+  <si>
+    <t>-7.14889053208308</t>
+  </si>
+  <si>
+    <t>40.0077322132428</t>
+  </si>
+  <si>
+    <t>-9.19456063486408</t>
+  </si>
+  <si>
+    <t>-5.85838531125264</t>
+  </si>
+  <si>
+    <t>41.3191952122571</t>
+  </si>
+  <si>
+    <t>-0.991610920912855</t>
+  </si>
+  <si>
+    <t>46.38749335084</t>
+  </si>
+  <si>
+    <t>43.388363485552</t>
+  </si>
+  <si>
+    <t>-23.9209739212368</t>
+  </si>
+  <si>
+    <t>-25.2048339055072</t>
+  </si>
+  <si>
+    <t>-30.0138978805907</t>
+  </si>
+  <si>
+    <t>-26.9385839261492</t>
+  </si>
+  <si>
+    <t>18.4393494725729</t>
+  </si>
+  <si>
+    <t>4.47925195311279</t>
+  </si>
+  <si>
+    <t>-0.265290358836554</t>
+  </si>
+  <si>
+    <t>2.82616641555524</t>
+  </si>
+  <si>
+    <t>48.3412237958865</t>
+  </si>
+  <si>
+    <t>0.840185706762245</t>
+  </si>
+  <si>
+    <t>3.92906278622457</t>
+  </si>
+  <si>
+    <t>49.423162388372</t>
+  </si>
+  <si>
+    <t>7.41666332398662</t>
+  </si>
+  <si>
+    <t>52.709239177891</t>
+  </si>
+  <si>
+    <t>49.2833166401053</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>46.7333015339765</t>
+  </si>
+  <si>
+    <t>47.9300023297263</t>
+  </si>
+  <si>
+    <t>52.1071897937773</t>
+  </si>
+  <si>
+    <t>48.8946635922404</t>
+  </si>
+  <si>
+    <t>2.55882352941176</t>
   </si>
 </sst>
 </file>

</xml_diff>